<commit_message>
Logistic phase characterization (not feasibility)
Static export cable has been 25% characterized
Dynamic Cable has been characterized
Driven Pile has been characterized
Drag Anchor has been characterized
Direct Anchor has been characterized
Suction Anchor has been characterized
Pile Anchor has been characterized
</commit_message>
<xml_diff>
--- a/src/databases/ouputs_electrical.xlsx
+++ b/src/databases/ouputs_electrical.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="collection point" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="74">
   <si>
     <t>id [-]</t>
   </si>
@@ -238,6 +238,15 @@
   </si>
   <si>
     <t>array</t>
+  </si>
+  <si>
+    <t>device001</t>
+  </si>
+  <si>
+    <t>device002</t>
+  </si>
+  <si>
+    <t>trench type [-]</t>
   </si>
 </sst>
 </file>
@@ -634,8 +643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -847,8 +856,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y4"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -973,14 +982,14 @@
       <c r="H2" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="I2" s="6">
-        <v>0</v>
+      <c r="I2" s="6" t="s">
+        <v>71</v>
       </c>
       <c r="M2" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="N2" s="6">
-        <v>0</v>
+      <c r="N2" s="6" t="s">
+        <v>72</v>
       </c>
       <c r="R2" s="6" t="s">
         <v>51</v>
@@ -1005,14 +1014,14 @@
       <c r="H3" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="I3" s="6">
-        <v>0</v>
+      <c r="I3" s="6" t="s">
+        <v>71</v>
       </c>
       <c r="M3" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="N3" s="6">
-        <v>0</v>
+      <c r="N3" s="6" t="s">
+        <v>72</v>
       </c>
       <c r="R3" s="6" t="s">
         <v>50</v>
@@ -1038,13 +1047,13 @@
         <v>53</v>
       </c>
       <c r="I4" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M4" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="N4" s="6">
-        <v>0</v>
+      <c r="N4" s="6" t="s">
+        <v>71</v>
       </c>
       <c r="R4" s="6" t="s">
         <v>56</v>
@@ -1064,7 +1073,7 @@
   <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:P16"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1707,10 +1716,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H130"/>
+  <dimension ref="A1:I130"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D130"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1723,10 +1732,11 @@
     <col min="6" max="6" width="17.85546875"/>
     <col min="7" max="7" width="20.7109375"/>
     <col min="8" max="8" width="15.140625"/>
-    <col min="9" max="1025" width="8.5703125"/>
+    <col min="9" max="9" width="16.85546875" customWidth="1"/>
+    <col min="10" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>38</v>
       </c>
@@ -1751,8 +1761,11 @@
       <c r="H1" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
@@ -1766,7 +1779,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1780,7 +1793,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1794,7 +1807,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1808,7 +1821,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -1822,7 +1835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2</v>
       </c>
@@ -1836,7 +1849,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2</v>
       </c>
@@ -1850,7 +1863,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2</v>
       </c>
@@ -1864,7 +1877,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2</v>
       </c>
@@ -1878,7 +1891,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2</v>
       </c>
@@ -1892,7 +1905,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2</v>
       </c>
@@ -1906,7 +1919,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2</v>
       </c>
@@ -1920,7 +1933,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2</v>
       </c>
@@ -1934,7 +1947,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2</v>
       </c>
@@ -1948,7 +1961,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2</v>
       </c>
@@ -3892,7 +3905,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="K40" sqref="K40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>